<commit_message>
Add ARWA and remaining resource stack
</commit_message>
<xml_diff>
--- a/data/sample_bs.xlsx
+++ b/data/sample_bs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreymarvel/Projects/bs_optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreymarvel/Projects/bs_optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AACC11-DF28-E642-96F8-6D3BB644AC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA780A-B2D5-234C-B3D2-8EE1A05C86B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15680" xr2:uid="{5975144E-CF9B-8442-B451-9396CF3D45DA}"/>
+    <workbookView xWindow="31960" yWindow="2220" windowWidth="27640" windowHeight="15680" activeTab="1" xr2:uid="{5975144E-CF9B-8442-B451-9396CF3D45DA}"/>
   </bookViews>
   <sheets>
     <sheet name="bs" sheetId="1" r:id="rId1"/>
     <sheet name="constraints" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Product</t>
   </si>
@@ -97,9 +97,6 @@
     <t>s_rwa</t>
   </si>
   <si>
-    <t>gsib</t>
-  </si>
-  <si>
     <t>business_loan_revolver</t>
   </si>
   <si>
@@ -152,6 +149,45 @@
   </si>
   <si>
     <t>commercial_loan_revolver</t>
+  </si>
+  <si>
+    <t>CET1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>total_capital</t>
+  </si>
+  <si>
+    <t>TLAC</t>
+  </si>
+  <si>
+    <t>SRWA</t>
+  </si>
+  <si>
+    <t>ARWA</t>
+  </si>
+  <si>
+    <t>prefs</t>
+  </si>
+  <si>
+    <t>sub_debt</t>
+  </si>
+  <si>
+    <t>senior_debt</t>
+  </si>
+  <si>
+    <t>CET1_resource</t>
+  </si>
+  <si>
+    <t>T1_resource</t>
+  </si>
+  <si>
+    <t>total_capital_resource</t>
+  </si>
+  <si>
+    <t>TLAC_resource</t>
   </si>
 </sst>
 </file>
@@ -159,16 +195,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0;\-#,##0;\-"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;\-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -205,12 +234,6 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri (Body)"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,32 +252,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,20 +588,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C859C2AE-61FB-4947-9EF3-3D4562E34A75}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -605,16 +634,21 @@
       <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -622,13 +656,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="6">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="D2" s="7">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="E2" s="7">
-        <v>-3000</v>
+        <v>-5000</v>
       </c>
       <c r="F2" s="7">
         <v>80</v>
@@ -636,20 +670,29 @@
       <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>0.2</v>
       </c>
-      <c r="I2" s="10">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="7"/>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12">
+        <v>0</v>
+      </c>
+      <c r="M2" s="12">
+        <v>0</v>
+      </c>
       <c r="N2" s="7"/>
       <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -658,13 +701,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="7">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7">
-        <v>-500</v>
+        <v>-1000</v>
       </c>
       <c r="F3" s="7">
         <v>150</v>
@@ -672,35 +715,44 @@
       <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>0.6</v>
       </c>
-      <c r="I3" s="10">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="7"/>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" s="12">
+        <v>0</v>
+      </c>
       <c r="N3" s="7"/>
       <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A27" si="0">A3+1</f>
+        <f t="shared" ref="A4:A30" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D4" s="7">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E4" s="7">
-        <v>-10000</v>
+        <v>-15000</v>
       </c>
       <c r="F4" s="7">
         <v>70</v>
@@ -708,20 +760,29 @@
       <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>0.3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>0.5</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="7"/>
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0</v>
+      </c>
       <c r="N4" s="7"/>
       <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -744,20 +805,29 @@
       <c r="G5" s="7">
         <v>1</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>0.3</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>0.5</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="7"/>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
       <c r="N5" s="7"/>
       <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -780,20 +850,29 @@
       <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>0.3</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>0.5</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="7"/>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
       <c r="N6" s="7"/>
       <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -816,20 +895,29 @@
       <c r="G7" s="7">
         <v>1</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>0.3</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>0.5</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="7"/>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
       <c r="N7" s="7"/>
       <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -852,20 +940,29 @@
       <c r="G8" s="7">
         <v>1</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>0.3</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>0.5</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="7"/>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
       <c r="N8" s="7"/>
       <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -874,7 +971,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="7">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D9" s="7">
         <v>20000</v>
@@ -888,20 +985,29 @@
       <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I9" s="10">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="7"/>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
       <c r="N9" s="7"/>
       <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -924,26 +1030,35 @@
       <c r="G10" s="7">
         <v>1</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>0.95</v>
       </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="7"/>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
       <c r="N10" s="7"/>
       <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>20000</v>
@@ -960,32 +1075,41 @@
       <c r="G11" s="7">
         <v>1</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>0.75</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>1.2</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="7"/>
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <v>0</v>
+      </c>
       <c r="N11" s="7"/>
       <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
-        <v>40000</v>
+        <v>55000</v>
       </c>
       <c r="D12" s="7">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E12" s="7">
         <v>-8500</v>
@@ -996,26 +1120,35 @@
       <c r="G12" s="7">
         <v>1</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>0.7</v>
       </c>
-      <c r="I12" s="10">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="7"/>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
       <c r="N12" s="7"/>
       <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="7">
         <v>40000</v>
@@ -1032,32 +1165,41 @@
       <c r="G13" s="7">
         <v>1</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>0.65</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="7"/>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
       <c r="N13" s="7"/>
       <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="D14" s="7">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E14" s="7">
         <v>-15000</v>
@@ -1068,20 +1210,29 @@
       <c r="G14" s="7">
         <v>1</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>0.6</v>
       </c>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="7"/>
+      <c r="I14" s="9">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
       <c r="N14" s="7"/>
       <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1104,26 +1255,35 @@
       <c r="G15" s="8">
         <v>1</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>0.4</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="7"/>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <v>0</v>
+      </c>
+      <c r="M15" s="12">
+        <v>0</v>
+      </c>
       <c r="N15" s="7"/>
       <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="8">
         <v>60000</v>
@@ -1140,26 +1300,35 @@
       <c r="G16" s="8">
         <v>1</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>0.5</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>0.6</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="7"/>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
       <c r="N16" s="7"/>
       <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8">
         <v>75000</v>
@@ -1176,20 +1345,29 @@
       <c r="G17" s="8">
         <v>1</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>0.35</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>0.5</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="7"/>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
       <c r="N17" s="7"/>
       <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1212,20 +1390,29 @@
       <c r="G18" s="8">
         <v>1</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>0.5</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>0.7</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="7"/>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
       <c r="N18" s="7"/>
       <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1248,26 +1435,35 @@
       <c r="G19" s="8">
         <v>1</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <v>0.05</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>0.05</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="7"/>
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12">
+        <v>0</v>
+      </c>
       <c r="N19" s="7"/>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8">
         <v>175000</v>
@@ -1284,26 +1480,35 @@
       <c r="G20" s="8">
         <v>-1</v>
       </c>
-      <c r="H20" s="11">
-        <v>0</v>
-      </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="7"/>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
       <c r="N20" s="7"/>
       <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8">
         <v>60000</v>
@@ -1320,26 +1525,35 @@
       <c r="G21" s="8">
         <v>-1</v>
       </c>
-      <c r="H21" s="11">
-        <v>0</v>
-      </c>
-      <c r="I21" s="11">
-        <v>0</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="7"/>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
+        <v>0</v>
+      </c>
       <c r="N21" s="7"/>
       <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8">
         <v>100000</v>
@@ -1356,26 +1570,35 @@
       <c r="G22" s="8">
         <v>-1</v>
       </c>
-      <c r="H22" s="11">
-        <v>0</v>
-      </c>
-      <c r="I22" s="11">
-        <v>0</v>
-      </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="7"/>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>0</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
       <c r="N22" s="7"/>
       <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="7"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="8">
         <v>20000</v>
@@ -1392,26 +1615,35 @@
       <c r="G23" s="8">
         <v>-1</v>
       </c>
-      <c r="H23" s="11">
-        <v>0</v>
-      </c>
-      <c r="I23" s="11">
-        <v>0</v>
-      </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="7"/>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12">
+        <v>0</v>
+      </c>
       <c r="N23" s="7"/>
       <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="7"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="8">
         <v>90500</v>
@@ -1428,26 +1660,35 @@
       <c r="G24" s="8">
         <v>-1</v>
       </c>
-      <c r="H24" s="11">
-        <v>0</v>
-      </c>
-      <c r="I24" s="11">
-        <v>0</v>
-      </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="7"/>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0</v>
+      </c>
       <c r="N24" s="7"/>
       <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="7"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="8">
         <v>42000</v>
@@ -1464,26 +1705,35 @@
       <c r="G25" s="8">
         <v>-1</v>
       </c>
-      <c r="H25" s="11">
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
-        <v>0</v>
-      </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="7"/>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12">
+        <v>0</v>
+      </c>
       <c r="N25" s="7"/>
       <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="7"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="8">
         <v>53000</v>
@@ -1500,26 +1750,35 @@
       <c r="G26" s="8">
         <v>-1</v>
       </c>
-      <c r="H26" s="11">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0</v>
-      </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="7"/>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
+        <v>0</v>
+      </c>
       <c r="N26" s="7"/>
       <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="7"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="8">
         <v>52500</v>
@@ -1528,7 +1787,7 @@
         <v>100000</v>
       </c>
       <c r="E27" s="8">
-        <v>-55000</v>
+        <v>-52500</v>
       </c>
       <c r="F27" s="8">
         <v>-1000</v>
@@ -1536,103 +1795,180 @@
       <c r="G27" s="8">
         <v>-1</v>
       </c>
-      <c r="H27" s="11">
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
-        <v>0</v>
-      </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="7"/>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+      <c r="J27" s="13">
+        <v>1</v>
+      </c>
+      <c r="K27" s="13">
+        <v>1</v>
+      </c>
+      <c r="L27" s="13">
+        <v>1</v>
+      </c>
+      <c r="M27" s="13">
+        <v>1</v>
+      </c>
       <c r="N27" s="7"/>
       <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="7"/>
+      <c r="P27" s="7"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="8">
+        <v>8000</v>
+      </c>
+      <c r="D28" s="8">
+        <v>13000</v>
+      </c>
+      <c r="E28" s="8">
+        <v>-7000</v>
+      </c>
+      <c r="F28" s="8">
+        <v>-650</v>
+      </c>
+      <c r="G28" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13">
+        <v>1</v>
+      </c>
+      <c r="L28" s="13">
+        <v>1</v>
+      </c>
+      <c r="M28" s="13">
+        <v>1</v>
+      </c>
       <c r="N28" s="7"/>
       <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="B29" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C29" s="8">
-        <f>SUM(C2:C19)</f>
-        <v>593000</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="7"/>
+        <v>11000</v>
+      </c>
+      <c r="D29" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E29" s="8">
+        <v>-9500</v>
+      </c>
+      <c r="F29" s="8">
+        <v>-200</v>
+      </c>
+      <c r="G29" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="13">
+        <v>0</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0</v>
+      </c>
+      <c r="L29" s="13">
+        <v>1</v>
+      </c>
+      <c r="M29" s="13">
+        <v>1</v>
+      </c>
       <c r="N29" s="7"/>
       <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="P29" s="7"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="B30" s="4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C30" s="8">
-        <f>SUM(C20:C27)</f>
-        <v>593000</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="7"/>
+        <v>43000</v>
+      </c>
+      <c r="D30" s="8">
+        <v>60000</v>
+      </c>
+      <c r="E30" s="8">
+        <v>-40000</v>
+      </c>
+      <c r="F30" s="8">
+        <v>-120</v>
+      </c>
+      <c r="G30" s="8">
+        <v>-1</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+      <c r="J30" s="13">
+        <v>0</v>
+      </c>
+      <c r="K30" s="13">
+        <v>0</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
+        <v>1</v>
+      </c>
       <c r="N30" s="7"/>
       <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" s="7"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
-      <c r="B31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="8">
-        <f>C29-C30</f>
-        <v>0</v>
-      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="9"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31" s="7"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1642,12 +1978,13 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="M32" s="7"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
@@ -1659,10 +1996,10 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
@@ -1675,10 +2012,10 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="10"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
+      <c r="M34" s="7"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
@@ -1691,49 +2028,179 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
+      <c r="M35" s="7"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="8">
+        <f>SUM(C2:C19)</f>
+        <v>655000</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
+      <c r="J36" s="10"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="B37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="8">
+        <f>SUM(C20:C30)</f>
+        <v>655000</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
+      <c r="J37" s="10"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="8">
+        <f>C36-C37</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J39" s="10"/>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J40" s="10"/>
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J41" s="10"/>
+      <c r="M41" s="8"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J42" s="10"/>
+      <c r="M42" s="8"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J43" s="10"/>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J44" s="10"/>
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M47" s="8"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M48" s="8"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M49" s="8"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C29:C30" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06FEFEE-149B-214C-ABE9-E743635185BD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>0.11</v>
+      </c>
+      <c r="C2">
+        <f>B2+ 0.015</f>
+        <v>0.125</v>
+      </c>
+      <c r="D2">
+        <f>C2+0.02</f>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E2">
+        <f>D2+0.08</f>
+        <v>0.22499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>0.11</v>
+      </c>
+      <c r="C3">
+        <f>B3+ 0.015</f>
+        <v>0.125</v>
+      </c>
+      <c r="D3">
+        <f>C3+0.02</f>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E3">
+        <f>D3+0.08</f>
+        <v>0.22499999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Successful minimize optimization w/ GSIB
</commit_message>
<xml_diff>
--- a/data/sample_bs.xlsx
+++ b/data/sample_bs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreymarvel/Projects/bs_optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F38DA5-F3B8-8E44-AD58-A4470DDDB06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1F082A-1291-D34F-B05D-169A0E126F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{5975144E-CF9B-8442-B451-9396CF3D45DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{5975144E-CF9B-8442-B451-9396CF3D45DA}"/>
   </bookViews>
   <sheets>
     <sheet name="bs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>Product</t>
   </si>
@@ -320,17 +320,24 @@
   <si>
     <t>synthetic_arwa_asset</t>
   </si>
+  <si>
+    <t>cet1_contr_per_balance</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;\-"/>
     <numFmt numFmtId="166" formatCode="0%;\-0%;\-"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
     <numFmt numFmtId="168" formatCode="0.0000%"/>
     <numFmt numFmtId="172" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="174" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -422,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -460,6 +467,7 @@
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,10 +786,10 @@
   <dimension ref="A1:DP322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Z15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z37" sqref="Z37"/>
+      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,9 +800,10 @@
     <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.83203125" customWidth="1"/>
     <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -856,7 +865,7 @@
         <v>56</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>58</v>
@@ -915,8 +924,11 @@
       <c r="AN1" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="AO1" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1051,8 +1063,12 @@
         <f>AM2*constraints!$B$5</f>
         <v>1.4447967251274234E-4</v>
       </c>
+      <c r="AO2" s="29">
+        <f>IFERROR(AN2/C2,0)</f>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -1188,10 +1204,14 @@
         <f>AM3*constraints!$B$5</f>
         <v>3.8527912670064624E-5</v>
       </c>
+      <c r="AO3" s="29">
+        <f t="shared" ref="AO3:AO41" si="1">IFERROR(AN3/C3,0)</f>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A41" si="1">A3+1</f>
+        <f t="shared" ref="A4:A41" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1325,10 +1345,14 @@
         <f>AM4*constraints!$B$5</f>
         <v>4.8159890837580775E-4</v>
       </c>
+      <c r="AO4" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1462,10 +1486,14 @@
         <f>AM5*constraints!$B$5</f>
         <v>1.4447967251274234E-4</v>
       </c>
+      <c r="AO5" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1599,10 +1627,14 @@
         <f>AM6*constraints!$B$5</f>
         <v>4.8159890837580777E-5</v>
       </c>
+      <c r="AO6" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1736,10 +1768,14 @@
         <f>AM7*constraints!$B$5</f>
         <v>1.9263956335032311E-4</v>
       </c>
+      <c r="AO7" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1873,10 +1909,14 @@
         <f>AM8*constraints!$B$5</f>
         <v>9.6319781675161553E-5</v>
       </c>
+      <c r="AO8" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2010,10 +2050,14 @@
         <f>AM9*constraints!$B$5</f>
         <v>5.7791869005096935E-4</v>
       </c>
+      <c r="AO9" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2147,10 +2191,14 @@
         <f>AM10*constraints!$B$5</f>
         <v>1.4447967251274234E-4</v>
       </c>
+      <c r="AO10" s="29">
+        <f t="shared" si="1"/>
+        <v>9.6319781675161553E-9</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2284,10 +2332,14 @@
         <f>AM11*constraints!$B$5</f>
         <v>2.7451137777421042E-4</v>
       </c>
+      <c r="AO11" s="29">
+        <f t="shared" si="1"/>
+        <v>1.3725568888710521E-8</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2421,10 +2473,14 @@
         <f>AM12*constraints!$B$5</f>
         <v>8.8734598868242585E-4</v>
       </c>
+      <c r="AO12" s="29">
+        <f t="shared" si="1"/>
+        <v>1.613356343058956E-8</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2558,10 +2614,14 @@
         <f>AM13*constraints!$B$5</f>
         <v>7.2239836256371166E-4</v>
       </c>
+      <c r="AO13" s="29">
+        <f t="shared" si="1"/>
+        <v>1.8059959064092791E-8</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2695,10 +2755,14 @@
         <f>AM14*constraints!$B$5</f>
         <v>2.094955251434764E-3</v>
       </c>
+      <c r="AO14" s="29">
+        <f t="shared" si="1"/>
+        <v>2.094955251434764E-8</v>
+      </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2832,10 +2896,14 @@
         <f>AM15*constraints!$B$5</f>
         <v>4.1224866556969142E-3</v>
       </c>
+      <c r="AO15" s="29">
+        <f t="shared" si="1"/>
+        <v>5.1531083196211427E-8</v>
+      </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2969,10 +3037,14 @@
         <f>AM16*constraints!$B$5</f>
         <v>3.3952723040494449E-3</v>
       </c>
+      <c r="AO16" s="29">
+        <f t="shared" si="1"/>
+        <v>5.6587871734157415E-8</v>
+      </c>
     </row>
     <row r="17" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -3106,10 +3178,14 @@
         <f>AM17*constraints!$B$5</f>
         <v>7.0975639121884666E-3</v>
       </c>
+      <c r="AO17" s="29">
+        <f t="shared" si="1"/>
+        <v>9.4634185495846227E-8</v>
+      </c>
     </row>
     <row r="18" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3243,10 +3319,14 @@
         <f>AM18*constraints!$B$5</f>
         <v>2.802905646747201E-3</v>
       </c>
+      <c r="AO18" s="29">
+        <f t="shared" si="1"/>
+        <v>9.3430188224906693E-8</v>
+      </c>
     </row>
     <row r="19" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3380,10 +3460,14 @@
         <f>AM19*constraints!$B$5</f>
         <v>1.8902757153750455E-3</v>
       </c>
+      <c r="AO19" s="29">
+        <f t="shared" si="1"/>
+        <v>1.8902757153750455E-7</v>
+      </c>
     </row>
     <row r="20" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -3517,10 +3601,14 @@
         <f>AM20*constraints!$B$5</f>
         <v>5.4300276919372326E-4</v>
       </c>
+      <c r="AO20" s="29">
+        <f t="shared" si="1"/>
+        <v>5.4300276919372323E-7</v>
+      </c>
     </row>
     <row r="21" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -3647,17 +3735,21 @@
         <v>0</v>
       </c>
       <c r="AM21" s="22">
-        <f t="shared" ref="AM21" si="2">SUM(AA21:AL21)</f>
+        <f t="shared" ref="AM21" si="3">SUM(AA21:AL21)</f>
         <v>0</v>
       </c>
       <c r="AN21" s="25">
         <f>AM21*constraints!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="AO21" s="29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -3789,12 +3881,16 @@
       </c>
       <c r="AN22" s="25">
         <f>AM22*constraints!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="AO22" s="29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -3926,12 +4022,16 @@
       </c>
       <c r="AN23" s="25">
         <f>AM23*constraints!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="AO23" s="29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -4063,12 +4163,16 @@
       </c>
       <c r="AN24" s="25">
         <f>AM24*constraints!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="AO24" s="29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -4202,8 +4306,10 @@
         <f>AM25*constraints!$B$5</f>
         <v>4.8159890837580775E-4</v>
       </c>
-      <c r="AO25" s="23"/>
-      <c r="AP25" s="23"/>
+      <c r="AO25" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790387E-8</v>
+      </c>
       <c r="AQ25" s="23"/>
       <c r="AR25" s="23"/>
       <c r="AS25" s="23"/>
@@ -4285,7 +4391,7 @@
     </row>
     <row r="26" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -4419,8 +4525,10 @@
         <f>AM26*constraints!$B$5</f>
         <v>0</v>
       </c>
-      <c r="AO26" s="23"/>
-      <c r="AP26" s="23"/>
+      <c r="AO26" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AQ26" s="23"/>
       <c r="AR26" s="23"/>
       <c r="AS26" s="23"/>
@@ -4502,7 +4610,7 @@
     </row>
     <row r="27" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -4636,8 +4744,10 @@
         <f>AM27*constraints!$B$5</f>
         <v>1.2039972709395194E-4</v>
       </c>
-      <c r="AO27" s="23"/>
-      <c r="AP27" s="23"/>
+      <c r="AO27" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790387E-8</v>
+      </c>
       <c r="AQ27" s="23"/>
       <c r="AR27" s="23"/>
       <c r="AS27" s="23"/>
@@ -4719,7 +4829,7 @@
     </row>
     <row r="28" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -4853,8 +4963,10 @@
         <f>AM28*constraints!$B$5</f>
         <v>0</v>
       </c>
-      <c r="AO28" s="23"/>
-      <c r="AP28" s="23"/>
+      <c r="AO28" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AQ28" s="23"/>
       <c r="AR28" s="23"/>
       <c r="AS28" s="23"/>
@@ -4936,7 +5048,7 @@
     </row>
     <row r="29" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -5070,8 +5182,10 @@
         <f>AM29*constraints!$B$5</f>
         <v>6.0199863546975968E-4</v>
       </c>
-      <c r="AO29" s="23"/>
-      <c r="AP29" s="23"/>
+      <c r="AO29" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790387E-8</v>
+      </c>
       <c r="AQ29" s="23"/>
       <c r="AR29" s="23"/>
       <c r="AS29" s="23"/>
@@ -5153,7 +5267,7 @@
     </row>
     <row r="30" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -5287,8 +5401,10 @@
         <f>AM30*constraints!$B$5</f>
         <v>4.093590721194366E-4</v>
       </c>
-      <c r="AO30" s="23"/>
-      <c r="AP30" s="23"/>
+      <c r="AO30" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790387E-8</v>
+      </c>
       <c r="AQ30" s="23"/>
       <c r="AR30" s="23"/>
       <c r="AS30" s="23"/>
@@ -5370,7 +5486,7 @@
     </row>
     <row r="31" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -5504,8 +5620,10 @@
         <f>AM31*constraints!$B$5</f>
         <v>4.093590721194366E-4</v>
       </c>
-      <c r="AO31" s="23"/>
-      <c r="AP31" s="23"/>
+      <c r="AO31" s="29">
+        <f t="shared" si="1"/>
+        <v>4.8159890837580775E-8</v>
+      </c>
       <c r="AQ31" s="23"/>
       <c r="AR31" s="23"/>
       <c r="AS31" s="23"/>
@@ -5587,7 +5705,7 @@
     </row>
     <row r="32" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -5721,8 +5839,10 @@
         <f>AM32*constraints!$B$5</f>
         <v>0</v>
       </c>
-      <c r="AO32" s="23"/>
-      <c r="AP32" s="23"/>
+      <c r="AO32" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AQ32" s="23"/>
       <c r="AR32" s="23"/>
       <c r="AS32" s="23"/>
@@ -5804,7 +5924,7 @@
     </row>
     <row r="33" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -5938,8 +6058,10 @@
         <f>AM33*constraints!$B$5</f>
         <v>2.8895934502548467E-4</v>
       </c>
-      <c r="AO33" s="23"/>
-      <c r="AP33" s="23"/>
+      <c r="AO33" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790391E-8</v>
+      </c>
       <c r="AQ33" s="23"/>
       <c r="AR33" s="23"/>
       <c r="AS33" s="23"/>
@@ -6021,7 +6143,7 @@
     </row>
     <row r="34" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -6155,8 +6277,10 @@
         <f>AM34*constraints!$B$5</f>
         <v>1.6855961793153272E-4</v>
       </c>
-      <c r="AO34" s="23"/>
-      <c r="AP34" s="23"/>
+      <c r="AO34" s="29">
+        <f t="shared" si="1"/>
+        <v>2.4079945418790387E-8</v>
+      </c>
       <c r="AQ34" s="23"/>
       <c r="AR34" s="23"/>
       <c r="AS34" s="23"/>
@@ -6238,7 +6362,7 @@
     </row>
     <row r="35" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -6372,8 +6496,10 @@
         <f>AM35*constraints!$B$5</f>
         <v>1.4447967251274234E-4</v>
       </c>
-      <c r="AO35" s="23"/>
-      <c r="AP35" s="23"/>
+      <c r="AO35" s="29">
+        <f t="shared" si="1"/>
+        <v>4.8159890837580781E-8</v>
+      </c>
       <c r="AQ35" s="23"/>
       <c r="AR35" s="23"/>
       <c r="AS35" s="23"/>
@@ -6455,7 +6581,7 @@
     </row>
     <row r="36" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -6589,8 +6715,10 @@
         <f>AM36*constraints!$B$5</f>
         <v>0</v>
       </c>
-      <c r="AO36" s="23"/>
-      <c r="AP36" s="23"/>
+      <c r="AO36" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AQ36" s="23"/>
       <c r="AR36" s="23"/>
       <c r="AS36" s="23"/>
@@ -6672,7 +6800,7 @@
     </row>
     <row r="37" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -6683,11 +6811,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="8">
-        <f t="shared" ref="D37:E37" si="3">D21</f>
+        <f t="shared" ref="D37:E37" si="4">D21</f>
         <v>0</v>
       </c>
       <c r="E37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F37" s="8">
@@ -6802,15 +6930,17 @@
         <v>0</v>
       </c>
       <c r="AM37" s="22">
-        <f t="shared" ref="AM37" si="4">SUM(AA37:AL37)</f>
+        <f t="shared" ref="AM37" si="5">SUM(AA37:AL37)</f>
         <v>0</v>
       </c>
       <c r="AN37" s="25">
         <f>AM37*constraints!$B$5</f>
         <v>0</v>
       </c>
-      <c r="AO37" s="23"/>
-      <c r="AP37" s="23"/>
+      <c r="AO37" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AQ37" s="23"/>
       <c r="AR37" s="23"/>
       <c r="AS37" s="23"/>
@@ -6892,7 +7022,7 @@
     </row>
     <row r="38" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -7026,8 +7156,10 @@
         <f>AM38*constraints!$B$5</f>
         <v>7.8019023156880856E-4</v>
       </c>
-      <c r="AO38" s="23"/>
-      <c r="AP38" s="23"/>
+      <c r="AO38" s="29">
+        <f t="shared" si="1"/>
+        <v>1.4447967251274232E-8</v>
+      </c>
       <c r="AQ38" s="23"/>
       <c r="AR38" s="23"/>
       <c r="AS38" s="23"/>
@@ -7109,7 +7241,7 @@
     </row>
     <row r="39" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -7243,8 +7375,10 @@
         <f>AM39*constraints!$B$5</f>
         <v>1.1558373801019386E-4</v>
       </c>
-      <c r="AO39" s="23"/>
-      <c r="AP39" s="23"/>
+      <c r="AO39" s="29">
+        <f t="shared" si="1"/>
+        <v>1.4447967251274232E-8</v>
+      </c>
       <c r="AQ39" s="23"/>
       <c r="AR39" s="23"/>
       <c r="AS39" s="23"/>
@@ -7326,7 +7460,7 @@
     </row>
     <row r="40" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -7460,8 +7594,10 @@
         <f>AM40*constraints!$B$5</f>
         <v>1.5892763976401656E-4</v>
       </c>
-      <c r="AO40" s="23"/>
-      <c r="AP40" s="23"/>
+      <c r="AO40" s="29">
+        <f t="shared" si="1"/>
+        <v>1.4447967251274234E-8</v>
+      </c>
       <c r="AQ40" s="23"/>
       <c r="AR40" s="23"/>
       <c r="AS40" s="23"/>
@@ -7543,7 +7679,7 @@
     </row>
     <row r="41" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -7677,8 +7813,10 @@
         <f>AM41*constraints!$B$5</f>
         <v>6.2126259180479194E-4</v>
       </c>
-      <c r="AO41" s="23"/>
-      <c r="AP41" s="23"/>
+      <c r="AO41" s="29">
+        <f t="shared" si="1"/>
+        <v>1.444796725127423E-8</v>
+      </c>
       <c r="AQ41" s="23"/>
       <c r="AR41" s="23"/>
       <c r="AS41" s="23"/>
@@ -7797,13 +7935,15 @@
       <c r="AJ42" s="23"/>
       <c r="AK42" s="23"/>
       <c r="AL42" s="23"/>
-      <c r="AM42" s="23"/>
+      <c r="AM42" s="22">
+        <f>SUM(AM2:AM41)</f>
+        <v>622.92499999999984</v>
+      </c>
       <c r="AN42" s="28">
         <f>SUM(AN2:AN41)</f>
         <v>3.0000000000000006E-2</v>
       </c>
-      <c r="AO42" s="23"/>
-      <c r="AP42" s="23"/>
+      <c r="AP42" s="28"/>
       <c r="AQ42" s="23"/>
       <c r="AR42" s="23"/>
       <c r="AS42" s="23"/>
@@ -7922,10 +8062,6 @@
       <c r="AJ43" s="23"/>
       <c r="AK43" s="23"/>
       <c r="AL43" s="23"/>
-      <c r="AM43" s="22">
-        <f>SUM(AM2:AM41)</f>
-        <v>622.92499999999984</v>
-      </c>
       <c r="AN43" s="23"/>
       <c r="AO43" s="23"/>
       <c r="AP43" s="23"/>
@@ -8014,7 +8150,10 @@
       <c r="C44" s="8"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="5">
+        <f>-SUMPRODUCT(F2:F41,C2:C41)/10000</f>
+        <v>-10545.75</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="12"/>
       <c r="I44" s="5">
@@ -8183,7 +8322,7 @@
       <c r="AK45" s="23"/>
       <c r="AL45" s="23"/>
       <c r="AM45" s="26">
-        <f>AM44/AM43</f>
+        <f>AM44/AM42</f>
         <v>4.8159890837580777E-5</v>
       </c>
       <c r="AN45" s="23"/>
@@ -41810,7 +41949,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>